<commit_message>
Updated Fam and Practice lists and folders
</commit_message>
<xml_diff>
--- a/repswitch_fam.xlsx
+++ b/repswitch_fam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8773DDB1-8218-45E8-AC67-3D7927DA35AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9E6DB8-32D2-438C-B481-AC1C356A7BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="600" windowWidth="16284" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="7764" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>image</t>
   </si>
@@ -234,13 +234,55 @@
   </si>
   <si>
     <t>REPSWITCH1_Fam/PICTURE_546.png</t>
+  </si>
+  <si>
+    <t>rana</t>
+  </si>
+  <si>
+    <t>nube</t>
+  </si>
+  <si>
+    <t>toro</t>
+  </si>
+  <si>
+    <t>gafas</t>
+  </si>
+  <si>
+    <t>reina</t>
+  </si>
+  <si>
+    <t>mesa</t>
+  </si>
+  <si>
+    <t>sirena</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_612.png</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_599.png</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_570.png</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_733.png</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_614.png</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_110.png</t>
+  </si>
+  <si>
+    <t>REPSWITCH1_Practice/PICTURE_12.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +304,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +319,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -317,16 +365,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,8 +563,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0096A52A-5BE6-44CE-8F3A-D6837A65D305}" name="Table1" displayName="Table1" ref="A1:B33" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="A1:B33" xr:uid="{0096A52A-5BE6-44CE-8F3A-D6837A65D305}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0096A52A-5BE6-44CE-8F3A-D6837A65D305}" name="Table1" displayName="Table1" ref="A1:B40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="A1:B40" xr:uid="{0096A52A-5BE6-44CE-8F3A-D6837A65D305}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{34B3F00C-5A8F-4E3A-99C8-A728A5DF5F8C}" name="image" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{6E34E39B-FEE1-4FCA-8F3D-1FF456769306}" name="correctAns" dataDxfId="0"/>
@@ -510,9 +574,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -550,9 +614,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,26 +649,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,26 +684,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -830,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097A394-F70B-4BA9-8F65-A485BAED673C}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,6 +1139,62 @@
         <v>9</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>